<commit_message>
Updated examples for USDM v3.13.0
</commit_message>
<xml_diff>
--- a/Documents/Examples/Alexion_NCT04573309_Wilsons/Alexion_NCT04573309_Wilsons.xlsx
+++ b/Documents/Examples/Alexion_NCT04573309_Wilsons/Alexion_NCT04573309_Wilsons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/Alexion_NCT04573309_Wilsons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1574A11-DECA-5246-9629-A3BC9479E247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CE072F-88AD-4842-8BF3-F2DF7F8A35D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="49200" windowHeight="25420" firstSheet="19" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="500" windowWidth="49200" windowHeight="25420" firstSheet="19" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3722" uniqueCount="1740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3738" uniqueCount="1749">
   <si>
     <t>name</t>
   </si>
@@ -7420,6 +7420,33 @@
   </si>
   <si>
     <t>@plannedAge/Range/@minValue/Quantity/value</t>
+  </si>
+  <si>
+    <t>AMEND_1</t>
+  </si>
+  <si>
+    <t>The first amendment</t>
+  </si>
+  <si>
+    <t>AMEND_2</t>
+  </si>
+  <si>
+    <t>AMEND_3</t>
+  </si>
+  <si>
+    <t>AMEND_4</t>
+  </si>
+  <si>
+    <t>The second amendment</t>
+  </si>
+  <si>
+    <t>The third amendment</t>
+  </si>
+  <si>
+    <t>The fourth amendment</t>
+  </si>
+  <si>
+    <t>Amendment 4</t>
   </si>
 </sst>
 </file>
@@ -15942,173 +15969,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" customWidth="1"/>
-    <col min="5" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" customWidth="1"/>
+    <col min="8" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>1623</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>1726</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>1627</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>1628</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>1629</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:11" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>1723</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>1622</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>1630</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D7" s="2"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D9" s="2"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18254,10 +18330,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF7CA68-BC48-5141-BEA0-B0ABEF929D94}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18268,7 +18344,7 @@
     <col min="4" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -18290,8 +18366,11 @@
       <c r="G1" s="14" t="s">
         <v>1616</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="14" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1617</v>
       </c>
@@ -18629,7 +18708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -18698,7 +18777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>